<commit_message>
updated queries in 6 failing ubc01 scripts
</commit_message>
<xml_diff>
--- a/InputFiles/TC21_Canine_StudyUBC-AllBreeds_StageOfDisease.xlsx
+++ b/InputFiles/TC21_Canine_StudyUBC-AllBreeds_StageOfDisease.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\updated code\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9F07D0-60E4-4F58-9FA2-ECC3611F2F53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E50751A-6B16-4A76-83CC-00FBC035B66B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -63,20 +63,6 @@
     <t>TC21_Canine_StudyUBC-AllBreeds_StageOfDisease_WebData.xlsx</t>
   </si>
   <si>
-    <t>MATCH (s:study)
-  MATCH (demo:demographic) 
-  MATCH (diag:diagnosis)
- MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-	WHERE s.clinical_study_designation IN ['UBC01'] and diag.stage_of_disease in [ 'T2N0M0', 'T2N1M0', 'T3N0M0', 'T3N0M1', 'T3N1M0', 'Not Applicable'] 
-OPTIONAL MATCH (s)&lt;-[:member_of]-(c:case)
-OPTIONAL MATCH (c)&lt;-[:of_case]-(samp:sample)&lt;-[:of_sample]-(f:file)
-RETURN 
-	count(DISTINCT(f)) as number_of_files , 
-	count(DISTINCT(samp)) as number_of_sample , 
-	count(DISTINCT(c.case_id)) as number_of_cases , 
-	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
@@ -131,6 +117,54 @@
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
         coalesce(diag.best_response, '') AS `Response to Treatment`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (p:program)&lt;--(s:study)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+      WHERE (size([]) = 0 OR s.clinical_study_designation IN [])
+        AND (s.study_disposition = 'Unrestricted')
+        AND s.clinical_study_designation IN ['UBC01']
+		 and diag.stage_of_disease in [ 'T2N0M0', 'T2N1M0', 'T3N0M0', 'T3N0M1', 'T3N1M0', 'Not Applicable'] 
+        AND (size([]) = 0 OR demo.sex IN [])
+        AND (size([]) = 0 OR demo.neutered_indicator IN [])
+        AND (size([]) = 0 OR diag.disease_term IN [])
+        AND (size([]) = 0 OR diag.primary_disease_site IN [])
+        AND (size([]) = 0 OR diag.stage_of_disease IN [])
+        AND (size([]) = 0 OR diag.best_response IN [])
+    OPTIONAL MATCH (c)--&gt;(co:cohort)
+    OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+    OPTIONAL MATCH (f)--&gt;(parent)
+    OPTIONAL MATCH (samp:sample)--&gt;(c)
+    OPTIONAL MATCH (samp)&lt;--(al:aliquot)
+    WITH DISTINCT c AS c, p, s, co, demo, diag, f, parent, samp, al
+      WHERE (size([]) = 0 OR samp.summarized_sample_type IN [])
+        AND (size([]) = 0 OR samp.specific_sample_pathology IN [])
+        AND (size([]) = 0 OR samp.sample_site IN [])
+        AND (size([]) = 0 OR head(labels(parent)) IN [])
+        AND (size([]) = 0 OR f.file_type IN [])
+        AND (size([]) = 0 OR f.file_format IN [])
+    WITH c.case_id AS case_id,
+         s.clinical_study_designation AS study_code,
+         s.clinical_study_type AS study_type,
+         co.cohort_description AS cohort,
+         demo.breed AS breed,
+         diag.disease_term AS diagnosis,
+         diag.stage_of_disease AS stage_of_disease,
+         diag.primary_disease_site AS disease_site,
+         demo.patient_age_at_enrollment AS age,
+         demo.sex AS sex,
+         demo.neutered_indicator AS neutered_status,
+         demo.weight AS weight,
+         diag.best_response AS response_to_treatment,
+         samp.sample_id AS sample_id,
+         f.uuid AS file_id,
+         al
+    RETURN
+COUNT(DISTINCT file_id) as number_of_files,
+COUNT(DISTINCT sample_id) as number_of_sample,
+COUNT(DISTINCT case_id) as number_of_cases,
+COUNT(DISTINCT study_code) as number_of_study,
+COUNT(DISTINCT al) as number_of_aliquot
+    </t>
   </si>
 </sst>
 </file>
@@ -502,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -531,15 +565,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -548,15 +582,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -565,15 +599,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>

</xml_diff>